<commit_message>
Updated database and made 404 take up more space on smaller devices.
</commit_message>
<xml_diff>
--- a/CSEC Prep.xlsx
+++ b/CSEC Prep.xlsx
@@ -7,7 +7,7 @@
     <sheet state="visible" name="chemistry" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="biology" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="physics" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="add_maths" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="add-maths" sheetId="5" r:id="rId8"/>
     <sheet state="visible" name="mathematics" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="311">
   <si>
     <t>mathematics</t>
   </si>
   <si>
-    <t>add_maths</t>
+    <t>add-maths</t>
   </si>
   <si>
     <t>biology</t>
@@ -573,10 +573,10 @@
     <t>Lenses</t>
   </si>
   <si>
-    <t>e-c</t>
-  </si>
-  <si>
-    <t>Electrical Conductors</t>
+    <t>c-e</t>
+  </si>
+  <si>
+    <t>Current Electricity</t>
   </si>
   <si>
     <t>e-s</t>
@@ -651,9 +651,6 @@
     <t>a-b-s, m-c-v</t>
   </si>
   <si>
-    <t>c-e</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -747,6 +744,12 @@
     <t>a-d</t>
   </si>
   <si>
+    <t>elec, m-c-v</t>
+  </si>
+  <si>
+    <t>poly, reac</t>
+  </si>
+  <si>
     <t>drug, r-g-e</t>
   </si>
   <si>
@@ -804,6 +807,9 @@
     <t>biod, n-c</t>
   </si>
   <si>
+    <t>e-f</t>
+  </si>
+  <si>
     <t>lens, m-q</t>
   </si>
   <si>
@@ -819,13 +825,10 @@
     <t>s-l-h, h-t</t>
   </si>
   <si>
-    <t>e-f</t>
-  </si>
-  <si>
     <t>quan, forc, mome</t>
   </si>
   <si>
-    <t>e-c, elec</t>
+    <t>c-e, elec</t>
   </si>
   <si>
     <t>s-h-c, s-l-h</t>
@@ -867,6 +870,21 @@
     <t>w-t-m, e-w</t>
   </si>
   <si>
+    <t>moti, mome</t>
+  </si>
+  <si>
+    <t>m-q, moti</t>
+  </si>
+  <si>
+    <t>cond, circ, e-s</t>
+  </si>
+  <si>
+    <t>c-e, w-t-m</t>
+  </si>
+  <si>
+    <t>e-q, tran</t>
+  </si>
+  <si>
     <t>alge, quad</t>
   </si>
   <si>
@@ -876,6 +894,9 @@
     <t>stat, prob</t>
   </si>
   <si>
+    <t>stas</t>
+  </si>
+  <si>
     <t>alge, meas</t>
   </si>
   <si>
@@ -922,6 +943,12 @@
   </si>
   <si>
     <t>r-f-g, meas</t>
+  </si>
+  <si>
+    <t>g-t, meas</t>
+  </si>
+  <si>
+    <t>r-f-h</t>
   </si>
 </sst>
 </file>
@@ -1902,10 +1929,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="M28" s="5" t="s">
+      <c r="M28" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="6" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2077,7 +2104,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>211</v>
+        <v>185</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>101</v>
@@ -2097,7 +2124,7 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>173</v>
@@ -2117,7 +2144,7 @@
         <v>2.0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>43</v>
@@ -2137,10 +2164,10 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="8">
@@ -2157,10 +2184,10 @@
         <v>2.0</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="9">
@@ -2177,7 +2204,7 @@
         <v>3.0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>117</v>
@@ -2197,7 +2224,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>125</v>
@@ -2217,7 +2244,7 @@
         <v>4.0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>91</v>
@@ -2277,7 +2304,7 @@
         <v>5.0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>131</v>
@@ -2320,7 +2347,7 @@
         <v>209</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17">
@@ -2337,7 +2364,7 @@
         <v>6.0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>167</v>
@@ -2357,7 +2384,7 @@
         <v>1.0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>101</v>
@@ -2377,7 +2404,7 @@
         <v>1.0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>111</v>
@@ -2397,7 +2424,7 @@
         <v>1.0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>155</v>
@@ -2417,7 +2444,7 @@
         <v>1.0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>101</v>
@@ -2460,7 +2487,7 @@
         <v>209</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24">
@@ -2477,7 +2504,7 @@
         <v>2.0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>91</v>
@@ -2517,7 +2544,7 @@
         <v>3.0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>125</v>
@@ -2537,7 +2564,7 @@
         <v>4.0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>71</v>
@@ -2580,7 +2607,7 @@
         <v>209</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="30">
@@ -2597,7 +2624,7 @@
         <v>5.0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>125</v>
@@ -2617,7 +2644,7 @@
         <v>6.0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>143</v>
@@ -2700,7 +2727,7 @@
         <v>209</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36">
@@ -2757,7 +2784,7 @@
         <v>3.0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>125</v>
@@ -2777,7 +2804,7 @@
         <v>3.0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>117</v>
@@ -2797,7 +2824,7 @@
         <v>3.0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>125</v>
@@ -2817,7 +2844,7 @@
         <v>4.0</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>53</v>
@@ -2917,7 +2944,7 @@
         <v>6.0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>143</v>
@@ -2977,7 +3004,7 @@
         <v>1.0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>173</v>
@@ -3017,7 +3044,7 @@
         <v>2.0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>53</v>
@@ -3037,7 +3064,7 @@
         <v>3.0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>117</v>
@@ -3057,7 +3084,7 @@
         <v>3.0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>131</v>
@@ -3080,7 +3107,7 @@
         <v>208</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55">
@@ -3157,7 +3184,7 @@
         <v>5.0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>71</v>
@@ -3197,7 +3224,7 @@
         <v>6.0</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>167</v>
@@ -3220,7 +3247,7 @@
         <v>208</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="62">
@@ -3240,7 +3267,7 @@
         <v>209</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63">
@@ -3257,7 +3284,7 @@
         <v>1.0</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>173</v>
@@ -3280,7 +3307,7 @@
         <v>208</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65">
@@ -3317,7 +3344,7 @@
         <v>2.0</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>53</v>
@@ -3337,10 +3364,10 @@
         <v>2.0</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68">
@@ -3377,10 +3404,10 @@
         <v>3.0</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="70">
@@ -3437,7 +3464,7 @@
         <v>5.0</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>143</v>
@@ -3477,7 +3504,7 @@
         <v>6.0</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>149</v>
@@ -3497,7 +3524,7 @@
         <v>6.0</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>71</v>
@@ -3557,7 +3584,7 @@
         <v>1.0</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>23</v>
@@ -3577,7 +3604,7 @@
         <v>1.0</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>173</v>
@@ -3597,7 +3624,7 @@
         <v>2.0</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>43</v>
@@ -3617,7 +3644,7 @@
         <v>2.0</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>53</v>
@@ -3657,7 +3684,7 @@
         <v>3.0</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>131</v>
@@ -3700,7 +3727,7 @@
         <v>209</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86">
@@ -3717,7 +3744,7 @@
         <v>4.0</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>143</v>
@@ -3737,7 +3764,7 @@
         <v>5.0</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>91</v>
@@ -3757,7 +3784,7 @@
         <v>6.0</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>149</v>
@@ -3780,7 +3807,7 @@
         <v>208</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90">
@@ -3817,7 +3844,7 @@
         <v>2.0</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>91</v>
@@ -3837,10 +3864,10 @@
         <v>2.0</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="93">
@@ -3857,7 +3884,7 @@
         <v>2.0</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>91</v>
@@ -3880,7 +3907,7 @@
         <v>208</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="95">
@@ -3900,7 +3927,7 @@
         <v>209</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96">
@@ -3940,7 +3967,7 @@
         <v>209</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98">
@@ -3957,7 +3984,7 @@
         <v>5.0</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>143</v>
@@ -3977,7 +4004,7 @@
         <v>6.0</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>161</v>
@@ -3997,10 +4024,250 @@
         <v>6.0</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B101" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C101" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D101" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B102" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C102" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D102" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B103" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D103" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B104" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D104" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B105" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C105" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D105" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B106" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C106" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D106" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C107" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D107" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B108" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C108" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D108" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B109" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C109" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D109" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B110" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C110" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D110" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B111" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C111" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D111" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B112" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C112" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D112" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4095,7 +4362,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>79</v>
@@ -4115,7 +4382,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>51</v>
@@ -4135,7 +4402,7 @@
         <v>3.0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>135</v>
@@ -4155,7 +4422,7 @@
         <v>3.0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>159</v>
@@ -4175,7 +4442,7 @@
         <v>4.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>109</v>
@@ -4195,10 +4462,10 @@
         <v>4.0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10">
@@ -4218,7 +4485,7 @@
         <v>208</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11">
@@ -4235,7 +4502,7 @@
         <v>5.0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>147</v>
@@ -4258,7 +4525,7 @@
         <v>208</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13">
@@ -4275,7 +4542,7 @@
         <v>6.0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>141</v>
@@ -4298,7 +4565,7 @@
         <v>208</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15">
@@ -4318,7 +4585,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16">
@@ -4335,7 +4602,7 @@
         <v>1.0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>69</v>
@@ -4355,7 +4622,7 @@
         <v>2.0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>11</v>
@@ -4375,7 +4642,7 @@
         <v>2.0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>165</v>
@@ -4395,7 +4662,7 @@
         <v>3.0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>141</v>
@@ -4478,7 +4745,7 @@
         <v>209</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24">
@@ -4518,7 +4785,7 @@
         <v>209</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26">
@@ -4538,7 +4805,7 @@
         <v>208</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27">
@@ -4555,7 +4822,7 @@
         <v>1.0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>69</v>
@@ -4635,7 +4902,7 @@
         <v>3.0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>135</v>
@@ -4655,7 +4922,7 @@
         <v>4.0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>141</v>
@@ -4715,10 +4982,10 @@
         <v>6.0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36">
@@ -4738,7 +5005,7 @@
         <v>208</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37">
@@ -4755,7 +5022,7 @@
         <v>1.0</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>21</v>
@@ -4775,7 +5042,7 @@
         <v>2.0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>79</v>
@@ -4798,7 +5065,7 @@
         <v>208</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40">
@@ -4818,7 +5085,7 @@
         <v>209</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41">
@@ -4835,7 +5102,7 @@
         <v>4.0</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>31</v>
@@ -4858,7 +5125,7 @@
         <v>208</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43">
@@ -4878,7 +5145,7 @@
         <v>209</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="44">
@@ -4895,7 +5162,7 @@
         <v>5.0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>165</v>
@@ -4955,7 +5222,7 @@
         <v>1.0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>165</v>
@@ -4975,7 +5242,7 @@
         <v>1.0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>79</v>
@@ -5015,10 +5282,10 @@
         <v>2.0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="51">
@@ -5058,7 +5325,7 @@
         <v>209</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53">
@@ -5095,7 +5362,7 @@
         <v>4.0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>147</v>
@@ -5115,7 +5382,7 @@
         <v>5.0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>41</v>
@@ -5135,7 +5402,7 @@
         <v>5.0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>31</v>
@@ -5158,7 +5425,7 @@
         <v>208</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="58">
@@ -5175,7 +5442,7 @@
         <v>6.0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>99</v>
@@ -5195,7 +5462,7 @@
         <v>1.0</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>69</v>
@@ -5215,7 +5482,7 @@
         <v>2.0</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>115</v>
@@ -5235,7 +5502,7 @@
         <v>2.0</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>147</v>
@@ -5255,7 +5522,7 @@
         <v>3.0</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F62" s="5" t="s">
         <v>51</v>
@@ -5275,7 +5542,7 @@
         <v>3.0</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>61</v>
@@ -5295,7 +5562,7 @@
         <v>3.0</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>51</v>
@@ -5315,7 +5582,7 @@
         <v>4.0</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>159</v>
@@ -5335,7 +5602,7 @@
         <v>5.0</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F66" s="5" t="s">
         <v>147</v>
@@ -5355,7 +5622,7 @@
         <v>6.0</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>141</v>
@@ -5375,7 +5642,7 @@
         <v>1.0</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>79</v>
@@ -5395,10 +5662,10 @@
         <v>2.0</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70">
@@ -5438,7 +5705,7 @@
         <v>209</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72">
@@ -5475,7 +5742,7 @@
         <v>4.0</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>61</v>
@@ -5495,7 +5762,7 @@
         <v>4.0</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>69</v>
@@ -5515,7 +5782,7 @@
         <v>5.0</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>89</v>
@@ -5559,6 +5826,266 @@
       </c>
       <c r="F77" s="5" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C78" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D78" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C79" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C80" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D80" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C81" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D81" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C82" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D82" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C83" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D83" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C84" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D84" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C85" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D85" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B86" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C86" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D86" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C87" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D87" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B88" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D88" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B89" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C89" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D89" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="5">
+        <v>2010.0</v>
+      </c>
+      <c r="B90" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C90" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D90" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -5610,10 +6137,10 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3">
@@ -5630,7 +6157,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>183</v>
@@ -5690,10 +6217,10 @@
         <v>3.0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7">
@@ -5710,10 +6237,10 @@
         <v>3.0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8">
@@ -5730,7 +6257,7 @@
         <v>4.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>145</v>
@@ -5750,7 +6277,7 @@
         <v>5.0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>45</v>
@@ -5770,7 +6297,7 @@
         <v>5.0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>65</v>
@@ -5790,7 +6317,7 @@
         <v>6.0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>79</v>
@@ -5810,7 +6337,7 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>196</v>
@@ -5830,7 +6357,7 @@
         <v>2.0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>157</v>
@@ -5850,7 +6377,7 @@
         <v>2.0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>169</v>
@@ -5870,7 +6397,7 @@
         <v>3.0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>201</v>
@@ -5890,7 +6417,7 @@
         <v>4.0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>65</v>
@@ -5933,7 +6460,7 @@
         <v>209</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19">
@@ -5950,7 +6477,7 @@
         <v>6.0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>183</v>
@@ -5970,7 +6497,7 @@
         <v>1.0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>201</v>
@@ -5990,7 +6517,7 @@
         <v>1.0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>199</v>
@@ -6013,7 +6540,7 @@
         <v>208</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23">
@@ -6050,7 +6577,7 @@
         <v>2.0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>73</v>
@@ -6090,7 +6617,7 @@
         <v>3.0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>139</v>
@@ -6130,7 +6657,7 @@
         <v>4.0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>157</v>
@@ -6152,8 +6679,8 @@
       <c r="E29" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>269</v>
+      <c r="F29" s="6" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="30">
@@ -6230,7 +6757,7 @@
         <v>1.0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>201</v>
@@ -6290,10 +6817,10 @@
         <v>2.0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
@@ -6373,7 +6900,7 @@
         <v>209</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41">
@@ -6430,7 +6957,7 @@
         <v>6.0</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>183</v>
@@ -6450,7 +6977,7 @@
         <v>1.0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>119</v>
@@ -6470,10 +6997,10 @@
         <v>1.0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46">
@@ -6513,7 +7040,7 @@
         <v>209</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="48">
@@ -6553,7 +7080,7 @@
         <v>209</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="50">
@@ -6593,7 +7120,7 @@
         <v>209</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52">
@@ -6633,7 +7160,7 @@
         <v>209</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54">
@@ -6650,7 +7177,7 @@
         <v>6.0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>201</v>
@@ -6670,7 +7197,7 @@
         <v>1.0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>45</v>
@@ -6690,10 +7217,10 @@
         <v>1.0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57">
@@ -6713,7 +7240,7 @@
         <v>208</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="58">
@@ -6733,7 +7260,7 @@
         <v>209</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="59">
@@ -6753,7 +7280,7 @@
         <v>208</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="60">
@@ -6773,7 +7300,7 @@
         <v>209</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="61">
@@ -6790,7 +7317,7 @@
         <v>4.0</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>73</v>
@@ -6812,7 +7339,7 @@
       <c r="E62" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="6" t="s">
         <v>185</v>
       </c>
     </row>
@@ -6833,7 +7360,7 @@
         <v>209</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="64">
@@ -6850,7 +7377,7 @@
         <v>6.0</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>201</v>
@@ -6870,7 +7397,7 @@
         <v>1.0</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>189</v>
@@ -6890,10 +7417,10 @@
         <v>1.0</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67">
@@ -6950,7 +7477,7 @@
         <v>3.0</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>55</v>
@@ -6970,7 +7497,7 @@
         <v>3.0</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>35</v>
@@ -6990,7 +7517,7 @@
         <v>3.0</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>93</v>
@@ -7053,7 +7580,7 @@
         <v>208</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75">
@@ -7073,7 +7600,7 @@
         <v>209</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76">
@@ -7093,7 +7620,7 @@
         <v>208</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="77">
@@ -7110,10 +7637,230 @@
         <v>6.0</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B78" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C78" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F78" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B79" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C79" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D79" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C80" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D80" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B81" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C81" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D81" s="6">
+        <v>2.0</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B82" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C82" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D82" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B83" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C83" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D83" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B84" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C84" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D84" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B85" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C85" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D85" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B86" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C86" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D86" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B87" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C87" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D87" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="5">
+        <v>2011.0</v>
+      </c>
+      <c r="B88" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D88" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -7188,7 +7935,7 @@
         <v>209</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4">
@@ -7205,7 +7952,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>39</v>
@@ -7285,7 +8032,7 @@
         <v>3.0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>67</v>
@@ -7305,7 +8052,7 @@
         <v>4.0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>77</v>
@@ -7325,7 +8072,7 @@
         <v>5.0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>87</v>
@@ -7345,7 +8092,7 @@
         <v>6.0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>97</v>
@@ -7365,7 +8112,7 @@
         <v>6.0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>97</v>
@@ -7485,7 +8232,7 @@
         <v>1.0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>39</v>
@@ -7545,7 +8292,7 @@
         <v>2.0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>19</v>
@@ -7565,7 +8312,7 @@
         <v>3.0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>59</v>
@@ -7585,7 +8332,7 @@
         <v>3.0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>67</v>
@@ -7605,7 +8352,7 @@
         <v>4.0</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>77</v>
@@ -7625,7 +8372,7 @@
         <v>5.0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>87</v>
@@ -7645,7 +8392,7 @@
         <v>6.0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>97</v>
@@ -7685,7 +8432,7 @@
         <v>7.0</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>121</v>
@@ -7705,7 +8452,7 @@
         <v>8.0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>107</v>
@@ -7725,7 +8472,7 @@
         <v>1.0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>9</v>
@@ -7745,7 +8492,7 @@
         <v>1.0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>39</v>
@@ -7787,8 +8534,8 @@
       <c r="E33" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>39</v>
+      <c r="F33" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="34">
@@ -7805,7 +8552,7 @@
         <v>2.0</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>49</v>
@@ -7865,7 +8612,7 @@
         <v>4.0</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>77</v>
@@ -7885,7 +8632,7 @@
         <v>5.0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>87</v>
@@ -7908,7 +8655,7 @@
         <v>208</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
     </row>
     <row r="40">
@@ -7925,7 +8672,7 @@
         <v>6.0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>97</v>
@@ -7985,7 +8732,7 @@
         <v>7.0</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>121</v>
@@ -8005,7 +8752,7 @@
         <v>8.0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>107</v>
@@ -8045,7 +8792,7 @@
         <v>1.0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>39</v>
@@ -8085,7 +8832,7 @@
         <v>2.0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>49</v>
@@ -8145,7 +8892,7 @@
         <v>4.0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>77</v>
@@ -8165,7 +8912,7 @@
         <v>5.0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>87</v>
@@ -8185,7 +8932,7 @@
         <v>6.0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>97</v>
@@ -8225,7 +8972,7 @@
         <v>7.0</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F55" s="5" t="s">
         <v>121</v>
@@ -8245,7 +8992,7 @@
         <v>8.0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>107</v>
@@ -8265,7 +9012,7 @@
         <v>1.0</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>9</v>
@@ -8285,7 +9032,7 @@
         <v>1.0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>39</v>
@@ -8305,7 +9052,7 @@
         <v>2.0</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>19</v>
@@ -8325,7 +9072,7 @@
         <v>2.0</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>49</v>
@@ -8385,7 +9132,7 @@
         <v>4.0</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>77</v>
@@ -8405,7 +9152,7 @@
         <v>5.0</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>87</v>
@@ -8425,7 +9172,7 @@
         <v>6.0</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>97</v>
@@ -8485,7 +9232,7 @@
         <v>7.0</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>121</v>
@@ -8505,7 +9252,7 @@
         <v>8.0</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>107</v>
@@ -8525,7 +9272,7 @@
         <v>1.0</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>9</v>
@@ -8567,8 +9314,8 @@
       <c r="E72" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F72" s="5" t="s">
-        <v>39</v>
+      <c r="F72" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="73">
@@ -8585,7 +9332,7 @@
         <v>2.0</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>49</v>
@@ -8605,7 +9352,7 @@
         <v>3.0</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>59</v>
@@ -8625,7 +9372,7 @@
         <v>4.0</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>77</v>
@@ -8645,7 +9392,7 @@
         <v>5.0</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>87</v>
@@ -8665,7 +9412,7 @@
         <v>6.0</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F77" s="5" t="s">
         <v>97</v>
@@ -8725,7 +9472,7 @@
         <v>7.0</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>57</v>
@@ -8745,7 +9492,7 @@
         <v>8.0</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>107</v>
@@ -8765,7 +9512,7 @@
         <v>1.0</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>9</v>
@@ -8785,7 +9532,7 @@
         <v>1.0</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>39</v>
@@ -8827,8 +9574,8 @@
       <c r="E85" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="F85" s="5" t="s">
-        <v>39</v>
+      <c r="F85" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="86">
@@ -8845,7 +9592,7 @@
         <v>2.0</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F86" s="5" t="s">
         <v>49</v>
@@ -8885,7 +9632,7 @@
         <v>3.0</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>67</v>
@@ -8905,7 +9652,7 @@
         <v>4.0</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>77</v>
@@ -8925,7 +9672,7 @@
         <v>5.0</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>87</v>
@@ -8945,7 +9692,7 @@
         <v>6.0</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>97</v>
@@ -8988,7 +9735,7 @@
         <v>209</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
     </row>
     <row r="94">
@@ -9005,9 +9752,269 @@
         <v>8.0</v>
       </c>
       <c r="E94" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C95" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D95" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B96" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C96" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D96" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B97" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C97" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D97" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C98" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D98" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C99" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D99" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E99" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F99" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B100" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C100" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D100" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B101" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C101" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D101" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B102" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C102" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D102" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B103" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C103" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D103" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B104" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D104" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B105" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C105" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D105" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B106" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C106" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D106" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="5">
+        <v>2012.0</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="C107" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D107" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F107" s="5" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9063,7 +10070,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>7</v>
@@ -9083,7 +10090,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>9</v>
@@ -9103,7 +10110,7 @@
         <v>2.0</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>9</v>
@@ -9123,7 +10130,7 @@
         <v>3.0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>85</v>
@@ -9143,7 +10150,7 @@
         <v>4.0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>75</v>
@@ -9203,7 +10210,7 @@
         <v>6.0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>47</v>
@@ -9226,7 +10233,7 @@
         <v>208</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11">
@@ -9263,10 +10270,10 @@
         <v>7.0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13">
@@ -9286,7 +10293,7 @@
         <v>208</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14">
@@ -9323,7 +10330,7 @@
         <v>8.0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>47</v>
@@ -9343,7 +10350,7 @@
         <v>9.0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>85</v>
@@ -9363,7 +10370,7 @@
         <v>10.0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>95</v>
@@ -9406,7 +10413,7 @@
         <v>209</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20">
@@ -9446,7 +10453,7 @@
         <v>209</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22">
@@ -9463,7 +10470,7 @@
         <v>2.0</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>9</v>
@@ -9506,7 +10513,7 @@
         <v>209</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25">
@@ -9523,7 +10530,7 @@
         <v>4.0</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>9</v>
@@ -9543,7 +10550,7 @@
         <v>4.0</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>75</v>
@@ -9563,7 +10570,7 @@
         <v>5.0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>57</v>
@@ -9606,7 +10613,7 @@
         <v>209</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="30">
@@ -9623,7 +10630,7 @@
         <v>7.0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>17</v>
@@ -9646,7 +10653,7 @@
         <v>208</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
     </row>
     <row r="32">
@@ -9666,7 +10673,7 @@
         <v>209</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
     </row>
     <row r="33">
@@ -9706,7 +10713,7 @@
         <v>209</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35">
@@ -9726,7 +10733,7 @@
         <v>208</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
     </row>
     <row r="36">
@@ -9786,7 +10793,7 @@
         <v>209</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
     </row>
     <row r="39">
@@ -9803,7 +10810,7 @@
         <v>2.0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>9</v>
@@ -9823,7 +10830,7 @@
         <v>3.0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>85</v>
@@ -9886,7 +10893,7 @@
         <v>208</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44">
@@ -9923,7 +10930,7 @@
         <v>6.0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>47</v>
@@ -9943,10 +10950,10 @@
         <v>7.0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47">
@@ -10003,7 +11010,7 @@
         <v>9.0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>85</v>
@@ -10023,7 +11030,7 @@
         <v>10.0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>95</v>
@@ -10063,7 +11070,7 @@
         <v>1.0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>27</v>
@@ -10083,7 +11090,7 @@
         <v>2.0</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>9</v>
@@ -10103,10 +11110,10 @@
         <v>2.0</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55">
@@ -10163,7 +11170,7 @@
         <v>4.0</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>75</v>
@@ -10183,7 +11190,7 @@
         <v>5.0</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F58" s="5" t="s">
         <v>85</v>
@@ -10203,7 +11210,7 @@
         <v>6.0</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>47</v>
@@ -10223,7 +11230,7 @@
         <v>7.0</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>57</v>
@@ -10243,10 +11250,10 @@
         <v>8.0</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="62">
@@ -10303,7 +11310,7 @@
         <v>10.0</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>85</v>
@@ -10323,7 +11330,7 @@
         <v>11.0</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>95</v>
@@ -10363,7 +11370,7 @@
         <v>1.0</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>27</v>
@@ -10383,7 +11390,7 @@
         <v>2.0</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F68" s="5" t="s">
         <v>9</v>
@@ -10443,7 +11450,7 @@
         <v>4.0</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>47</v>
@@ -10463,7 +11470,7 @@
         <v>5.0</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F72" s="5" t="s">
         <v>85</v>
@@ -10483,7 +11490,7 @@
         <v>6.0</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>75</v>
@@ -10503,7 +11510,7 @@
         <v>7.0</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F74" s="5" t="s">
         <v>57</v>
@@ -10523,7 +11530,7 @@
         <v>8.0</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>105</v>
@@ -10583,7 +11590,7 @@
         <v>10.0</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>85</v>
@@ -10603,7 +11610,7 @@
         <v>11.0</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F79" s="5" t="s">
         <v>95</v>
@@ -10663,7 +11670,7 @@
         <v>2.0</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>9</v>
@@ -10683,10 +11690,10 @@
         <v>2.0</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
     </row>
     <row r="84">
@@ -10703,7 +11710,7 @@
         <v>2.0</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>9</v>
@@ -10763,7 +11770,7 @@
         <v>4.0</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>75</v>
@@ -10806,7 +11813,7 @@
         <v>209</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90">
@@ -10823,7 +11830,7 @@
         <v>5.0</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F90" s="5" t="s">
         <v>47</v>
@@ -10883,7 +11890,7 @@
         <v>7.0</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>57</v>
@@ -10926,7 +11933,7 @@
         <v>209</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="96">
@@ -10983,7 +11990,7 @@
         <v>10.0</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>85</v>
@@ -11003,7 +12010,7 @@
         <v>11.0</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>95</v>
@@ -11023,7 +12030,7 @@
         <v>1.0</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>7</v>
@@ -11043,7 +12050,7 @@
         <v>1.0</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>27</v>
@@ -11066,7 +12073,7 @@
         <v>208</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
     </row>
     <row r="103">
@@ -11083,7 +12090,7 @@
         <v>2.0</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>9</v>
@@ -11143,7 +12150,7 @@
         <v>4.0</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>47</v>
@@ -11163,7 +12170,7 @@
         <v>5.0</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>85</v>
@@ -11183,7 +12190,7 @@
         <v>6.0</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>75</v>
@@ -11203,7 +12210,7 @@
         <v>7.0</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>57</v>
@@ -11223,7 +12230,7 @@
         <v>8.0</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>105</v>
@@ -11246,7 +12253,7 @@
         <v>153</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
     </row>
     <row r="112">
@@ -11286,7 +12293,7 @@
         <v>209</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114">
@@ -11303,7 +12310,7 @@
         <v>10.0</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F114" s="5" t="s">
         <v>85</v>
@@ -11323,9 +12330,349 @@
         <v>11.0</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F115" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B116" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C116" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D116" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B117" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C117" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D117" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B118" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C118" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D118" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B119" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C119" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D119" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B120" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C120" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D120" s="5">
+        <v>3.0</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B121" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C121" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D121" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B122" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C122" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D122" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B123" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C123" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D123" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B124" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C124" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D124" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B125" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C125" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D125" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B126" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C126" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D126" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B127" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C127" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D127" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B128" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C128" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D128" s="6">
+        <v>8.0</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B129" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C129" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D129" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B130" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C130" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D130" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B131" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C131" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D131" s="5">
+        <v>10.0</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="5">
+        <v>2013.0</v>
+      </c>
+      <c r="B132" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="C132" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="D132" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="E132" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F132" s="5" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>